<commit_message>
Activities have been completed: The interview_dates column has been separated into day, month and year columns, and additional data was added to assess the default year used by Excel.
</commit_message>
<xml_diff>
--- a/DataCarpentry_DatesAsDataActivity.xlsx
+++ b/DataCarpentry_DatesAsDataActivity.xlsx
@@ -1,24 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ebecker/Box Sync/Carpentry_repos/datacarpentry-lessons/socialsci/spreadsheets-socialsci/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emily/Hunt-Exercises/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAF7688-8A43-A64F-8F8C-3872D8CC4635}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11320" yWindow="2640" windowWidth="27760" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="7460" yWindow="460" windowWidth="25600" windowHeight="14840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DD_MM_YEAR" sheetId="1" r:id="rId1"/>
     <sheet name="MM_DD_YEAR" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="24">
   <si>
     <t>interview_date</t>
   </si>
@@ -91,12 +98,21 @@
   </si>
   <si>
     <t>mabatipitched</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
@@ -136,11 +152,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -150,6 +167,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -417,365 +437,559 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.33203125" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="3"/>
-    <col min="2" max="2" width="17.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="22.33203125" style="2"/>
+    <col min="1" max="4" width="22.33203125" style="3"/>
+    <col min="5" max="5" width="17.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="22.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="B2" s="4">
+        <f>DAY(A2)</f>
+        <v>17</v>
+      </c>
+      <c r="C2" s="4">
+        <f>MONTH(A2)</f>
+        <v>11</v>
+      </c>
+      <c r="D2" s="4">
+        <f>YEAR(A2)</f>
+        <v>2016</v>
+      </c>
+      <c r="E2" s="2">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="4">
+        <f t="shared" ref="B3:B16" si="0">DAY(A3)</f>
+        <v>17</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:C16" si="1">MONTH(A3)</f>
+        <v>11</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D16" si="2">YEAR(A3)</f>
+        <v>2016</v>
+      </c>
+      <c r="E3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
+      <c r="C4" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="2"/>
+        <v>2016</v>
+      </c>
+      <c r="E4" s="2">
+        <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2">
+        <v>8</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="2"/>
+        <v>2016</v>
+      </c>
+      <c r="E5" s="2">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="2">
+        <v>12</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="4">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="2"/>
+        <v>2016</v>
+      </c>
+      <c r="E6" s="2">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2">
         <v>6</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="H6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="4">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="2"/>
+        <v>2016</v>
+      </c>
+      <c r="E7" s="2">
         <v>53</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2">
         <v>19</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="4">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="2"/>
+        <v>2016</v>
+      </c>
+      <c r="E8" s="2">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2">
+        <v>8</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="2"/>
+        <v>2016</v>
+      </c>
+      <c r="E9" s="2">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="2">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2">
+        <v>8</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="2"/>
+        <v>2016</v>
+      </c>
+      <c r="E10" s="2">
         <v>21</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="2">
-        <v>10</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2">
+        <v>10</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C11" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="2"/>
+        <v>2016</v>
+      </c>
+      <c r="E11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="2">
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2">
         <v>2</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="2"/>
+        <v>2016</v>
+      </c>
+      <c r="E12" s="2">
         <v>48</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="F12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="2">
         <v>7</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="B13" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="2"/>
+        <v>2016</v>
+      </c>
+      <c r="E13" s="2">
+        <v>12</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="2">
         <v>6</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C14" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="2"/>
+        <v>2016</v>
+      </c>
+      <c r="E14" s="2">
         <v>6</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="F14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="2">
         <v>6</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2">
-        <v>12</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="2">
+      <c r="B15" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="2"/>
+        <v>2016</v>
+      </c>
+      <c r="E15" s="2">
+        <v>12</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="2">
         <v>4</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>12</v>
+      <c r="H15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>43786</v>
+      </c>
+      <c r="B16" s="4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="2"/>
+        <v>2019</v>
       </c>
     </row>
   </sheetData>
@@ -784,7 +998,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>